<commit_message>
Organised Full Item list
</commit_message>
<xml_diff>
--- a/Magical_items_Minor.xlsx
+++ b/Magical_items_Minor.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane.donohue\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seang\Desktop\vendorGen WinForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3911AC-DC2A-42EB-8953-EABAAE0E6D3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,17 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="214">
   <si>
     <t>Item</t>
   </si>
@@ -674,12 +670,15 @@
   </si>
   <si>
     <t>Siegebreakers Knuckles</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -935,15 +934,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F101" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F101" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Roll" dataDxfId="5"/>
-    <tableColumn id="2" name="Item" dataDxfId="4"/>
-    <tableColumn id="3" name="Rarity" dataDxfId="3"/>
-    <tableColumn id="4" name="Name" dataDxfId="2"/>
-    <tableColumn id="5" name="Details" dataDxfId="1"/>
-    <tableColumn id="6" name="Attument" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Roll" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rarity" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Details" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Attument" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1245,25 +1244,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="84.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="84.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1303,7 +1302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1359,9 +1358,11 @@
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1377,9 +1378,11 @@
       <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1392,9 +1395,11 @@
       <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1408,7 +1413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1418,9 +1423,11 @@
       <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1430,9 +1437,11 @@
       <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1456,9 +1465,11 @@
       <c r="E12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1468,9 +1479,11 @@
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1498,7 +1511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1508,9 +1521,11 @@
       <c r="E16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1521,10 +1536,10 @@
         <v>41</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1535,10 +1550,10 @@
         <v>43</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1548,9 +1563,11 @@
       <c r="E19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1560,9 +1577,11 @@
       <c r="E20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1572,9 +1591,11 @@
       <c r="E21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1584,9 +1605,11 @@
       <c r="E22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1596,9 +1619,11 @@
       <c r="E23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="5" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1608,9 +1633,11 @@
       <c r="E24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1620,9 +1647,11 @@
       <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1632,9 +1661,11 @@
       <c r="E26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1648,7 +1679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1662,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1672,9 +1703,11 @@
       <c r="E29" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F29" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1684,9 +1717,11 @@
       <c r="E30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1696,9 +1731,11 @@
       <c r="E31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1708,9 +1745,11 @@
       <c r="E32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F32" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1720,9 +1759,11 @@
       <c r="E33" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F33" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1732,9 +1773,11 @@
       <c r="E34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F34" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1748,7 +1791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1762,7 +1805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1772,9 +1815,11 @@
       <c r="E37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F37" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1788,7 +1833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1798,9 +1843,11 @@
       <c r="E39" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1810,9 +1857,11 @@
       <c r="E40" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F40" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1826,7 +1875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1840,7 +1889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1850,9 +1899,11 @@
       <c r="E43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F43" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -1862,9 +1913,11 @@
       <c r="E44" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F44" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1874,9 +1927,11 @@
       <c r="E45" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -1890,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -1900,9 +1955,11 @@
       <c r="E47" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -1916,7 +1973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -1930,7 +1987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -1940,9 +1997,11 @@
       <c r="E50" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F50" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -1952,9 +2011,11 @@
       <c r="E51" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F51" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -1964,9 +2025,11 @@
       <c r="E52" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F52" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -1976,9 +2039,11 @@
       <c r="E53" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F53" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1992,7 +2057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -2002,9 +2067,11 @@
       <c r="E55" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F55" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -2014,9 +2081,11 @@
       <c r="E56" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F56" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -2026,9 +2095,11 @@
       <c r="E57" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F57" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -2038,9 +2109,11 @@
       <c r="E58" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F58" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -2054,7 +2127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -2068,7 +2141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -2078,9 +2151,11 @@
       <c r="E61" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F61" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -2090,9 +2165,11 @@
       <c r="E62" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F62" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -2106,7 +2183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -2116,9 +2193,11 @@
       <c r="E64" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F64" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -2132,7 +2211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -2146,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -2160,7 +2239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -2174,7 +2253,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -2184,9 +2263,11 @@
       <c r="E69" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="F69" s="6"/>
-    </row>
-    <row r="70" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F69" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -2200,7 +2281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -2214,7 +2295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -2228,7 +2309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -2238,9 +2319,11 @@
       <c r="E73" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F73" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -2250,9 +2333,11 @@
       <c r="E74" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="F74" s="6"/>
-    </row>
-    <row r="75" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F74" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -2266,7 +2351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -2276,9 +2361,11 @@
       <c r="E76" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F76" s="6"/>
-    </row>
-    <row r="77" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F76" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -2292,7 +2379,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -2306,7 +2393,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -2320,7 +2407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -2330,9 +2417,11 @@
       <c r="E80" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F80" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -2346,7 +2435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -2360,7 +2449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -2374,7 +2463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -2388,7 +2477,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -2402,7 +2491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -2416,7 +2505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -2426,9 +2515,11 @@
       <c r="E87" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F87" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -2442,7 +2533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -2456,7 +2547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -2470,7 +2561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -2480,9 +2571,11 @@
       <c r="E91" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F91" s="6"/>
-    </row>
-    <row r="92" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F91" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -2492,9 +2585,11 @@
       <c r="E92" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F92" s="6"/>
-    </row>
-    <row r="93" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F92" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -2504,9 +2599,11 @@
       <c r="E93" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F93" s="6"/>
-    </row>
-    <row r="94" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="F93" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -2520,7 +2617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -2530,9 +2627,11 @@
       <c r="E95" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="F95" s="6"/>
-    </row>
-    <row r="96" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F95" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -2542,9 +2641,11 @@
       <c r="E96" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="F96" s="6"/>
-    </row>
-    <row r="97" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F96" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -2554,9 +2655,11 @@
       <c r="E97" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="F97" s="6"/>
-    </row>
-    <row r="98" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F97" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -2570,7 +2673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -2584,7 +2687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -2598,7 +2701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -2608,7 +2711,9 @@
       <c r="E101" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F101" s="6"/>
+      <c r="F101" s="6" t="s">
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2620,14 +2725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>